<commit_message>
redid the infrastructure of search and changed back check and forward check to fit
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylo\Code\minesweeper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED5B706-9EDB-464F-860E-085AB3E71BB5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DA3BC0-E9CC-4A09-909C-F87A7D1C82BF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{ACEBBD04-204E-4560-B85E-0FB554B332B5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Solo Testing</t>
   </si>
@@ -74,6 +74,15 @@
   <si>
     <t>stopped for memory</t>
   </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>BC and FC</t>
+  </si>
+  <si>
+    <t>reduced the number of function calls</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +108,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -118,15 +127,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A32E22-72BC-4D65-ABF3-F045DE473E1A}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U24" sqref="U24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,18 +508,32 @@
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -480,8 +546,36 @@
       <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -503,8 +597,62 @@
       <c r="G3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -526,8 +674,62 @@
       <c r="G4">
         <v>62.375999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>1000</v>
+      </c>
+      <c r="M4">
+        <v>259.65300000000002</v>
+      </c>
+      <c r="N4">
+        <v>0.72</v>
+      </c>
+      <c r="O4">
+        <v>5002</v>
+      </c>
+      <c r="P4">
+        <v>589</v>
+      </c>
+      <c r="Q4">
+        <v>7.4470000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0.311</v>
+      </c>
+      <c r="T4">
+        <v>100</v>
+      </c>
+      <c r="U4">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="V4">
+        <v>0.65</v>
+      </c>
+      <c r="W4" s="4">
+        <v>3095</v>
+      </c>
+      <c r="X4" s="5">
+        <v>1818</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>5.431</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="AA4" s="4">
+        <v>1385</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>196</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>54.924999999999997</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0.316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -549,8 +751,41 @@
       <c r="G5">
         <v>38.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T5">
+        <v>100</v>
+      </c>
+      <c r="U5">
+        <v>11.247999999999999</v>
+      </c>
+      <c r="V5">
+        <v>0.82</v>
+      </c>
+      <c r="W5" s="4">
+        <v>3952</v>
+      </c>
+      <c r="X5" s="5">
+        <v>2389</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>7.25</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>1659</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>336</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>68.587000000000003</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -572,8 +807,41 @@
       <c r="G6">
         <v>94.26</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T6">
+        <v>100</v>
+      </c>
+      <c r="U6">
+        <v>25.969000000000001</v>
+      </c>
+      <c r="V6">
+        <v>0.76</v>
+      </c>
+      <c r="W6" s="4">
+        <v>8103</v>
+      </c>
+      <c r="X6" s="5">
+        <v>4616</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>14.769</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>4275</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>458</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>190.74299999999999</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0.28899999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -595,8 +863,41 @@
       <c r="G7">
         <v>15.651999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <v>100</v>
+      </c>
+      <c r="U7">
+        <v>8.91</v>
+      </c>
+      <c r="V7">
+        <v>0.69</v>
+      </c>
+      <c r="W7" s="4">
+        <v>2717</v>
+      </c>
+      <c r="X7" s="5">
+        <v>1573</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>4.4569999999999999</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>1352</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>217</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>51.228000000000002</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -618,8 +919,41 @@
       <c r="G8">
         <v>23.364000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T8" s="9">
+        <v>100</v>
+      </c>
+      <c r="U8" s="9">
+        <v>247.636</v>
+      </c>
+      <c r="V8" s="9">
+        <v>0.62</v>
+      </c>
+      <c r="W8" s="10">
+        <v>74786</v>
+      </c>
+      <c r="X8" s="11">
+        <v>37375</v>
+      </c>
+      <c r="Y8" s="11">
+        <v>126.10599999999999</v>
+      </c>
+      <c r="Z8" s="11">
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="AA8" s="10">
+        <v>48043</v>
+      </c>
+      <c r="AB8" s="11">
+        <v>297</v>
+      </c>
+      <c r="AC8" s="11">
+        <v>1995.001</v>
+      </c>
+      <c r="AD8" s="11">
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1000</v>
       </c>
@@ -641,8 +975,44 @@
       <c r="G9">
         <v>24.768000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T9">
+        <v>100</v>
+      </c>
+      <c r="U9">
+        <v>10.659000000000001</v>
+      </c>
+      <c r="V9">
+        <v>0.54</v>
+      </c>
+      <c r="W9" s="4">
+        <v>2895</v>
+      </c>
+      <c r="X9" s="5">
+        <v>1693</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>5.2089999999999996</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>1485</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>278</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>65.033000000000001</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1000</v>
       </c>
@@ -664,8 +1034,41 @@
       <c r="G10">
         <v>133.946</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T10">
+        <v>100</v>
+      </c>
+      <c r="U10">
+        <v>22.259</v>
+      </c>
+      <c r="V10">
+        <v>0.73</v>
+      </c>
+      <c r="W10" s="4">
+        <v>6649</v>
+      </c>
+      <c r="X10" s="5">
+        <v>3531</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>12.089</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>4038</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>315</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>164.44</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -687,8 +1090,41 @@
       <c r="G11">
         <v>44.932000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T11">
+        <v>100</v>
+      </c>
+      <c r="U11">
+        <v>7.5380000000000003</v>
+      </c>
+      <c r="V11">
+        <v>0.67</v>
+      </c>
+      <c r="W11" s="4">
+        <v>2437</v>
+      </c>
+      <c r="X11" s="5">
+        <v>1419</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>3.8879999999999999</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>1211</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>181</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>41.204999999999998</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1000</v>
       </c>
@@ -710,8 +1146,41 @@
       <c r="G12">
         <v>14.257</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T12">
+        <v>100</v>
+      </c>
+      <c r="U12">
+        <v>7.2889999999999997</v>
+      </c>
+      <c r="V12">
+        <v>0.7</v>
+      </c>
+      <c r="W12" s="4">
+        <v>2423</v>
+      </c>
+      <c r="X12" s="5">
+        <v>1432</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>3.9319999999999999</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>0.317</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>1118</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>169</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>38.435000000000002</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1000</v>
       </c>
@@ -733,8 +1202,41 @@
       <c r="G13">
         <v>110.023</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T13">
+        <v>100</v>
+      </c>
+      <c r="U13">
+        <v>12.294</v>
+      </c>
+      <c r="V13">
+        <v>0.84</v>
+      </c>
+      <c r="W13" s="4">
+        <v>4883</v>
+      </c>
+      <c r="X13" s="5">
+        <v>2810</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>8.42</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>2291</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>268</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>77.256</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <f>AVERAGE(B4:B13)</f>
         <v>172.51240000000001</v>
@@ -759,13 +1261,114 @@
         <f t="shared" si="0"/>
         <v>56.217799999999997</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <v>200</v>
+      </c>
+      <c r="U14">
+        <v>31.553000000000001</v>
+      </c>
+      <c r="V14">
+        <v>0.67</v>
+      </c>
+      <c r="W14" s="4">
+        <v>5554</v>
+      </c>
+      <c r="X14" s="5">
+        <v>3095</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>2805</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>365</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>108.011</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>0.26200000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="T15">
+        <v>200</v>
+      </c>
+      <c r="U15">
+        <v>18.754999999999999</v>
+      </c>
+      <c r="V15">
+        <v>0.84</v>
+      </c>
+      <c r="W15" s="4">
+        <v>3392</v>
+      </c>
+      <c r="X15" s="5">
+        <v>1951</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>5.1959999999999997</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>0.311</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>1668</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>231</v>
+      </c>
+      <c r="AC15" s="5">
+        <v>56.335999999999999</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T16">
+        <v>200</v>
+      </c>
+      <c r="U16">
+        <v>14.552</v>
+      </c>
+      <c r="V16">
+        <v>0.6</v>
+      </c>
+      <c r="W16" s="4">
+        <v>2608</v>
+      </c>
+      <c r="X16" s="5">
+        <v>1537</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>4.649</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>1211</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>186</v>
+      </c>
+      <c r="AC16" s="5">
+        <v>40.536000000000001</v>
+      </c>
+      <c r="AD16" s="5">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1000</v>
       </c>
@@ -787,8 +1390,41 @@
       <c r="G17">
         <v>0.31900000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T17">
+        <v>200</v>
+      </c>
+      <c r="U17">
+        <v>25.832000000000001</v>
+      </c>
+      <c r="V17">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="W17" s="4">
+        <v>4811</v>
+      </c>
+      <c r="X17" s="5">
+        <v>2775</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>7.7350000000000003</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>2256</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>198</v>
+      </c>
+      <c r="AC17" s="5">
+        <v>86.22</v>
+      </c>
+      <c r="AD17" s="5">
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1000</v>
       </c>
@@ -810,8 +1446,41 @@
       <c r="G18">
         <v>0.32400000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T18">
+        <v>200</v>
+      </c>
+      <c r="U18">
+        <v>53.930999999999997</v>
+      </c>
+      <c r="V18">
+        <v>0.77</v>
+      </c>
+      <c r="W18" s="4">
+        <v>9045</v>
+      </c>
+      <c r="X18" s="5">
+        <v>5295</v>
+      </c>
+      <c r="Y18" s="5">
+        <v>21.588999999999999</v>
+      </c>
+      <c r="Z18" s="5">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>3728</v>
+      </c>
+      <c r="AB18" s="5">
+        <v>470</v>
+      </c>
+      <c r="AC18" s="5">
+        <v>196.11099999999999</v>
+      </c>
+      <c r="AD18" s="5">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1000</v>
       </c>
@@ -833,8 +1502,41 @@
       <c r="G19">
         <v>0.318</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T19">
+        <v>400</v>
+      </c>
+      <c r="U19">
+        <v>133.755</v>
+      </c>
+      <c r="V19">
+        <v>0.75</v>
+      </c>
+      <c r="W19" s="4">
+        <v>9884</v>
+      </c>
+      <c r="X19" s="5">
+        <v>5654</v>
+      </c>
+      <c r="Y19" s="5">
+        <v>20.173999999999999</v>
+      </c>
+      <c r="Z19" s="5">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>4699</v>
+      </c>
+      <c r="AB19" s="5">
+        <v>1138</v>
+      </c>
+      <c r="AC19" s="5">
+        <v>251.21899999999999</v>
+      </c>
+      <c r="AD19" s="5">
+        <v>0.27700000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1000</v>
       </c>
@@ -859,8 +1561,41 @@
       <c r="H20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T20">
+        <v>400</v>
+      </c>
+      <c r="U20">
+        <v>56.277000000000001</v>
+      </c>
+      <c r="V20">
+        <v>0.7</v>
+      </c>
+      <c r="W20" s="4">
+        <v>4635</v>
+      </c>
+      <c r="X20" s="5">
+        <v>2726</v>
+      </c>
+      <c r="Y20" s="5">
+        <v>10.215999999999999</v>
+      </c>
+      <c r="Z20" s="5">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>1968</v>
+      </c>
+      <c r="AB20" s="5">
+        <v>331</v>
+      </c>
+      <c r="AC20" s="5">
+        <v>90.438000000000002</v>
+      </c>
+      <c r="AD20" s="5">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -885,8 +1620,41 @@
       <c r="H21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T21">
+        <v>400</v>
+      </c>
+      <c r="U21">
+        <v>91.201999999999998</v>
+      </c>
+      <c r="V21">
+        <v>0.65</v>
+      </c>
+      <c r="W21" s="4">
+        <v>6834</v>
+      </c>
+      <c r="X21" s="5">
+        <v>3826</v>
+      </c>
+      <c r="Y21" s="5">
+        <v>12.38</v>
+      </c>
+      <c r="Z21" s="5">
+        <v>0.34</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>3785</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>324</v>
+      </c>
+      <c r="AC21" s="5">
+        <v>166.75800000000001</v>
+      </c>
+      <c r="AD21" s="5">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1000</v>
       </c>
@@ -911,8 +1679,41 @@
       <c r="H22" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T22">
+        <v>400</v>
+      </c>
+      <c r="U22">
+        <v>165.14699999999999</v>
+      </c>
+      <c r="V22">
+        <v>0.66</v>
+      </c>
+      <c r="W22" s="4">
+        <v>11214</v>
+      </c>
+      <c r="X22" s="5">
+        <v>5767</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>22.042000000000002</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>7156</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>314</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>315.548</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>0.307</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1000</v>
       </c>
@@ -934,8 +1735,41 @@
       <c r="G23">
         <v>1.3029999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="T23">
+        <v>400</v>
+      </c>
+      <c r="U23">
+        <v>232.71799999999999</v>
+      </c>
+      <c r="V23">
+        <v>0.7</v>
+      </c>
+      <c r="W23" s="4">
+        <v>15670</v>
+      </c>
+      <c r="X23" s="5">
+        <v>8598</v>
+      </c>
+      <c r="Y23" s="5">
+        <v>34.159999999999997</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="AA23" s="4">
+        <v>8713</v>
+      </c>
+      <c r="AB23" s="5">
+        <v>308</v>
+      </c>
+      <c r="AC23" s="5">
+        <v>452.798</v>
+      </c>
+      <c r="AD23" s="5">
+        <v>0.28199999999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1000</v>
       </c>
@@ -958,7 +1792,7 @@
         <v>1.2629999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1000</v>
       </c>
@@ -981,7 +1815,7 @@
         <v>1.1859999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <f>AVERAGE(B17:B25)</f>
         <v>437.35822222222225</v>
@@ -1007,7 +1841,7 @@
         <v>0.91833333333333345</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>31.536000000000001</v>
       </c>
@@ -1027,7 +1861,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>68.298000000000002</v>
       </c>
@@ -1047,7 +1881,7 @@
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>148.27699999999999</v>
       </c>
@@ -1067,7 +1901,7 @@
         <v>0.28899999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>315.72500000000002</v>
       </c>
@@ -1090,7 +1924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>55.72</v>
       </c>
@@ -1211,6 +2045,10 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AA2:AE2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>